<commit_message>
updated flap sizing code
fixed aspect ratio calc for horizontal tail to fix lift slope
</commit_message>
<xml_diff>
--- a/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
+++ b/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tysonc/Documents/GitHub/433_design_problem/drag_buildup/derivatives/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tysonc/Documents/GitHub/443_design_problem/drag_buildup_flap_sizing/derivatives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F87177-C805-CE4E-83F5-15872100B7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520CD605-1D1F-834B-8D18-936D4EC2C101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57820" yWindow="500" windowWidth="10980" windowHeight="28300" xr2:uid="{FADF4127-3137-4FB6-88FA-242C48EF07EE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34480" windowHeight="21580" xr2:uid="{FADF4127-3137-4FB6-88FA-242C48EF07EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Input Equations" sheetId="3" r:id="rId1"/>
@@ -1315,8 +1315,8 @@
   <dimension ref="A1:G154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
+      <pane ySplit="3" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2739,8 +2739,8 @@
         <v>154</v>
       </c>
       <c r="C110" s="1">
-        <f>C111/C108</f>
-        <v>0.31097560975609756</v>
+        <f>C111^2/C108</f>
+        <v>3.9649390243902438</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
update dragbuildup excel file
to reflect the correct MAC of the wing
</commit_message>
<xml_diff>
--- a/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
+++ b/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tysonc/Documents/GitHub/443_design_problem/drag_buildup_flap_sizing/derivatives/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thais\Documents\GitHub\443_design_problem\drag_buildup_flap_sizing\derivatives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520CD605-1D1F-834B-8D18-936D4EC2C101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2C0812-FC36-411F-817B-1BD37447726A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34480" windowHeight="21580" xr2:uid="{FADF4127-3137-4FB6-88FA-242C48EF07EE}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{FADF4127-3137-4FB6-88FA-242C48EF07EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Input Equations" sheetId="3" r:id="rId1"/>
@@ -1315,20 +1315,20 @@
   <dimension ref="A1:G154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C111" sqref="C111"/>
+      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="21" t="s">
         <v>4</v>
       </c>
@@ -1336,7 +1336,7 @@
       <c r="C2" s="22"/>
       <c r="D2" s="23"/>
     </row>
-    <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>108</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>143</v>
       </c>
@@ -1446,7 +1446,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>152</v>
       </c>
@@ -1460,25 +1460,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="18" t="s">
         <v>53</v>
       </c>
@@ -1486,7 +1486,7 @@
       <c r="C15" s="19"/>
       <c r="D15" s="20"/>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
@@ -1536,14 +1536,13 @@
         <v>33</v>
       </c>
       <c r="C19" s="5">
-        <f>((2/3)*( (C16+C17-( (C16*C17)/(C16+C17) ))/(1+(C17/C16)) ) + C18)/2</f>
-        <v>4.653945374968437</v>
+        <v>6.1353</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -1558,7 +1557,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
@@ -1573,7 +1572,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1588,7 +1587,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -1617,7 +1616,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1631,7 +1630,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -1645,7 +1644,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>59</v>
       </c>
@@ -1659,7 +1658,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>112</v>
       </c>
@@ -1674,7 +1673,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>113</v>
       </c>
@@ -1689,7 +1688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>115</v>
       </c>
@@ -1704,7 +1703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>116</v>
       </c>
@@ -1719,7 +1718,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>117</v>
       </c>
@@ -1734,7 +1733,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>121</v>
       </c>
@@ -1749,7 +1748,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>122</v>
       </c>
@@ -1764,7 +1763,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>123</v>
       </c>
@@ -1779,7 +1778,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>124</v>
       </c>
@@ -1794,7 +1793,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>130</v>
       </c>
@@ -1806,7 +1805,7 @@
       </c>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>132</v>
       </c>
@@ -1820,7 +1819,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>142</v>
       </c>
@@ -1832,7 +1831,7 @@
       </c>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>146</v>
       </c>
@@ -1847,19 +1846,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="1"/>
       <c r="B41" s="6"/>
       <c r="C41" s="5"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A42" s="1"/>
       <c r="B42" s="6"/>
       <c r="C42" s="5"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A43" s="18" t="s">
         <v>64</v>
       </c>
@@ -1867,7 +1866,7 @@
       <c r="C43" s="19"/>
       <c r="D43" s="20"/>
     </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
@@ -1881,7 +1880,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
@@ -1895,7 +1894,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
@@ -1909,7 +1908,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -1923,7 +1922,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
@@ -1937,7 +1936,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="1"/>
       <c r="B49" s="5" t="s">
         <v>30</v>
@@ -1948,29 +1947,29 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C50" s="1">
         <f>0.225*C19</f>
-        <v>1.0471377093678984</v>
+        <v>1.3804425</v>
       </c>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C51" s="1">
         <f>0.225*C19</f>
-        <v>1.0471377093678984</v>
+        <v>1.3804425</v>
       </c>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>90</v>
       </c>
@@ -1984,7 +1983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>91</v>
       </c>
@@ -1998,7 +1997,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>95</v>
       </c>
@@ -2012,7 +2011,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>96</v>
       </c>
@@ -2026,7 +2025,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>224</v>
       </c>
@@ -2043,7 +2042,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>168</v>
       </c>
@@ -2057,7 +2056,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>170</v>
       </c>
@@ -2071,7 +2070,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A59" s="7" t="s">
         <v>172</v>
       </c>
@@ -2083,7 +2082,7 @@
       </c>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>174</v>
       </c>
@@ -2098,7 +2097,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>176</v>
       </c>
@@ -2120,7 +2119,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>179</v>
       </c>
@@ -2135,7 +2134,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A63" s="1" t="s">
         <v>181</v>
       </c>
@@ -2150,7 +2149,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A64" s="18" t="s">
         <v>184</v>
       </c>
@@ -2158,7 +2157,7 @@
       <c r="C64" s="19"/>
       <c r="D64" s="20"/>
     </row>
-    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="10" t="s">
         <v>5</v>
       </c>
@@ -2172,7 +2171,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>185</v>
       </c>
@@ -2187,13 +2186,13 @@
         <v>183</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="1:4" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A68" s="24" t="s">
         <v>187</v>
       </c>
@@ -2201,7 +2200,7 @@
       <c r="C68" s="25"/>
       <c r="D68" s="26"/>
     </row>
-    <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A69" s="2" t="s">
         <v>5</v>
       </c>
@@ -2215,7 +2214,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
         <v>188</v>
       </c>
@@ -2230,7 +2229,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
         <v>189</v>
       </c>
@@ -2245,7 +2244,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A72" s="24" t="s">
         <v>192</v>
       </c>
@@ -2253,37 +2252,37 @@
       <c r="C72" s="25"/>
       <c r="D72" s="26"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
       <c r="D73" s="13"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
       <c r="D74" s="13"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A78" s="24" t="s">
         <v>85</v>
       </c>
@@ -2291,7 +2290,7 @@
       <c r="C78" s="25"/>
       <c r="D78" s="26"/>
     </row>
-    <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
         <v>16</v>
       </c>
@@ -2306,7 +2305,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
         <v>17</v>
       </c>
@@ -2321,7 +2320,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
         <v>78</v>
       </c>
@@ -2335,7 +2334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
         <v>43</v>
       </c>
@@ -2350,7 +2349,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="39.4" x14ac:dyDescent="0.45">
       <c r="A83" s="8" t="s">
         <v>45</v>
       </c>
@@ -2365,7 +2364,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" s="9" t="s">
         <v>65</v>
       </c>
@@ -2379,7 +2378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
         <v>34</v>
       </c>
@@ -2394,7 +2393,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
         <v>15</v>
       </c>
@@ -2409,7 +2408,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
         <v>62</v>
       </c>
@@ -2423,7 +2422,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
         <v>63</v>
       </c>
@@ -2437,7 +2436,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
         <v>41</v>
       </c>
@@ -2452,7 +2451,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
         <v>68</v>
       </c>
@@ -2466,7 +2465,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
         <v>92</v>
       </c>
@@ -2480,7 +2479,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
         <v>94</v>
       </c>
@@ -2494,7 +2493,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" ht="16.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
         <v>194</v>
       </c>
@@ -2508,7 +2507,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
         <v>113</v>
       </c>
@@ -2523,7 +2522,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
         <v>115</v>
       </c>
@@ -2538,7 +2537,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="s">
         <v>116</v>
       </c>
@@ -2553,7 +2552,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="s">
         <v>117</v>
       </c>
@@ -2568,7 +2567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="s">
         <v>121</v>
       </c>
@@ -2583,7 +2582,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A99" s="1" t="s">
         <v>122</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
         <v>123</v>
       </c>
@@ -2613,7 +2612,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
         <v>124</v>
       </c>
@@ -2628,7 +2627,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A102" s="1" t="s">
         <v>130</v>
       </c>
@@ -2642,7 +2641,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A103" s="1" t="s">
         <v>131</v>
       </c>
@@ -2654,7 +2653,7 @@
       </c>
       <c r="D103" s="1"/>
     </row>
-    <row r="104" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A104" s="1" t="s">
         <v>218</v>
       </c>
@@ -2667,7 +2666,7 @@
       </c>
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A105" s="18" t="s">
         <v>86</v>
       </c>
@@ -2675,7 +2674,7 @@
       <c r="C105" s="19"/>
       <c r="D105" s="20"/>
     </row>
-    <row r="106" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
         <v>16</v>
       </c>
@@ -2690,7 +2689,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
         <v>17</v>
       </c>
@@ -2705,7 +2704,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A108" s="9" t="s">
         <v>155</v>
       </c>
@@ -2719,7 +2718,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A109" s="1" t="s">
         <v>43</v>
       </c>
@@ -2731,7 +2730,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A110" s="1" t="s">
         <v>151</v>
       </c>
@@ -2746,7 +2745,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A111" s="1" t="s">
         <v>157</v>
       </c>
@@ -2760,7 +2759,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" ht="39.4" x14ac:dyDescent="0.45">
       <c r="A112" s="8" t="s">
         <v>45</v>
       </c>
@@ -2772,7 +2771,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A113" s="1" t="s">
         <v>44</v>
       </c>
@@ -2786,7 +2785,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A114" s="1" t="s">
         <v>160</v>
       </c>
@@ -2800,7 +2799,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A115" s="7" t="s">
         <v>164</v>
       </c>
@@ -2814,7 +2813,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A116" s="1" t="s">
         <v>162</v>
       </c>
@@ -2824,7 +2823,7 @@
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A117" s="1" t="s">
         <v>34</v>
       </c>
@@ -2832,7 +2831,7 @@
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A118" s="1" t="s">
         <v>15</v>
       </c>
@@ -2840,7 +2839,7 @@
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A119" s="1" t="s">
         <v>62</v>
       </c>
@@ -2855,7 +2854,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A120" s="1" t="s">
         <v>63</v>
       </c>
@@ -2870,7 +2869,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A121" s="1" t="s">
         <v>41</v>
       </c>
@@ -2885,7 +2884,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="16.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A122" s="1" t="s">
         <v>82</v>
       </c>
@@ -2899,7 +2898,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A123" s="1" t="s">
         <v>83</v>
       </c>
@@ -2913,7 +2912,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A124" s="1" t="s">
         <v>97</v>
       </c>
@@ -2927,7 +2926,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A125" s="1" t="s">
         <v>89</v>
       </c>
@@ -2942,7 +2941,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A126" s="1" t="s">
         <v>100</v>
       </c>
@@ -2956,7 +2955,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A127" s="1" t="s">
         <v>101</v>
       </c>
@@ -2968,7 +2967,7 @@
       </c>
       <c r="D127" s="1"/>
     </row>
-    <row r="128" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A128" s="1" t="s">
         <v>151</v>
       </c>
@@ -2983,7 +2982,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" ht="114" x14ac:dyDescent="0.45">
       <c r="A129" s="1" t="s">
         <v>131</v>
       </c>
@@ -2997,7 +2996,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A130" s="1" t="s">
         <v>113</v>
       </c>
@@ -3012,7 +3011,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A131" s="1" t="s">
         <v>115</v>
       </c>
@@ -3027,7 +3026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" ht="16.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A132" s="1" t="s">
         <v>116</v>
       </c>
@@ -3042,7 +3041,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A133" s="1" t="s">
         <v>117</v>
       </c>
@@ -3057,7 +3056,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A134" s="1" t="s">
         <v>121</v>
       </c>
@@ -3072,7 +3071,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A135" s="1" t="s">
         <v>122</v>
       </c>
@@ -3087,7 +3086,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A136" s="1" t="s">
         <v>123</v>
       </c>
@@ -3102,7 +3101,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A137" s="1" t="s">
         <v>124</v>
       </c>
@@ -3117,7 +3116,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A138" s="1" t="s">
         <v>130</v>
       </c>
@@ -3129,7 +3128,7 @@
       </c>
       <c r="D138" s="1"/>
     </row>
-    <row r="139" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A139" s="1" t="s">
         <v>219</v>
       </c>
@@ -3142,25 +3141,25 @@
       </c>
       <c r="D139" s="1"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
     </row>
-    <row r="142" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
     </row>
-    <row r="143" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A143" s="18" t="s">
         <v>102</v>
       </c>
@@ -3168,7 +3167,7 @@
       <c r="C143" s="19"/>
       <c r="D143" s="20"/>
     </row>
-    <row r="144" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A144" s="1" t="s">
         <v>100</v>
       </c>
@@ -3180,7 +3179,7 @@
       </c>
       <c r="D144" s="1"/>
     </row>
-    <row r="145" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A145" s="1" t="s">
         <v>135</v>
       </c>
@@ -3194,7 +3193,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A146" s="1" t="s">
         <v>136</v>
       </c>
@@ -3208,7 +3207,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A147" s="1" t="s">
         <v>140</v>
       </c>
@@ -3222,7 +3221,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A148" s="1" t="s">
         <v>139</v>
       </c>
@@ -3239,31 +3238,31 @@
         <v>222</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
     </row>
-    <row r="152" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
     </row>
-    <row r="153" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A153" s="18" t="s">
         <v>149</v>
       </c>
@@ -3271,7 +3270,7 @@
       <c r="C153" s="19"/>
       <c r="D153" s="20"/>
     </row>
-    <row r="154" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A154" s="1" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
updated flap sizing,  drag buildup plotting
flap sizing now uses sea level conditions,

mainfunction plots different configuration polars
</commit_message>
<xml_diff>
--- a/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
+++ b/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bravo_4e3\OneDrive\Documents\GitHub\443_design_problem\drag_buildup_flap_sizing\derivatives\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tysonc/Documents/GitHub/443_design_problem/drag_buildup_flap_sizing/derivatives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092FEF67-9392-472B-BB3A-D41863F1E4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2871D903-69F0-7C40-B8C7-F363F7B20757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{FADF4127-3137-4FB6-88FA-242C48EF07EE}"/>
+    <workbookView xWindow="9120" yWindow="500" windowWidth="43640" windowHeight="28300" xr2:uid="{FADF4127-3137-4FB6-88FA-242C48EF07EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Input Equations" sheetId="3" r:id="rId1"/>
@@ -1402,20 +1402,20 @@
   <dimension ref="A1:G172"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F116" sqref="F116"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.234375" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.64453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="2" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>4</v>
       </c>
@@ -1423,7 +1423,7 @@
       <c r="C2" s="23"/>
       <c r="D2" s="24"/>
     </row>
-    <row r="3" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>108</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>143</v>
       </c>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>152</v>
       </c>
@@ -1547,25 +1547,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>53</v>
       </c>
@@ -1573,7 +1573,7 @@
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>59</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>112</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>113</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>115</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>116</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>117</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>121</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>122</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>123</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>124</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>130</v>
       </c>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>132</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>142</v>
       </c>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>146</v>
       </c>
@@ -1933,19 +1933,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="6"/>
       <c r="C41" s="5"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="6"/>
       <c r="C42" s="5"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>64</v>
       </c>
@@ -1953,7 +1953,7 @@
       <c r="C43" s="20"/>
       <c r="D43" s="21"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="5" t="s">
         <v>30</v>
@@ -2034,7 +2034,7 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
         <v>31</v>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
         <v>32</v>
@@ -2056,7 +2056,7 @@
       </c>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>90</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>91</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>95</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>96</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>224</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>168</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>170</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="86" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>172</v>
       </c>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="1:7" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>174</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>176</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>179</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:7" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>181</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="19" t="s">
         <v>184</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="C64" s="20"/>
       <c r="D64" s="21"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
         <v>5</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="43" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>185</v>
       </c>
@@ -2273,13 +2273,13 @@
         <v>183</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="1:4" ht="16.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:4" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
         <v>187</v>
       </c>
@@ -2287,7 +2287,7 @@
       <c r="C68" s="26"/>
       <c r="D68" s="27"/>
     </row>
-    <row r="69" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>5</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>188</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>189</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="25" t="s">
         <v>192</v>
       </c>
@@ -2339,37 +2339,37 @@
       <c r="C72" s="26"/>
       <c r="D72" s="27"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
       <c r="D73" s="13"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
       <c r="D74" s="13"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
     </row>
-    <row r="77" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>85</v>
       </c>
@@ -2377,7 +2377,7 @@
       <c r="C78" s="20"/>
       <c r="D78" s="21"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>16</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>17</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>78</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>43</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="39" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
         <v>45</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="9" t="s">
         <v>65</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>34</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>15</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>62</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>63</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>41</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>68</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>92</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>94</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="16.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>194</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>113</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>115</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>116</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>117</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>121</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>122</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>123</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>124</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>130</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>131</v>
       </c>
@@ -2740,7 +2740,7 @@
       </c>
       <c r="D103" s="1"/>
     </row>
-    <row r="104" spans="1:4" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>218</v>
       </c>
@@ -2753,7 +2753,7 @@
       </c>
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="19" t="s">
         <v>86</v>
       </c>
@@ -2761,7 +2761,7 @@
       <c r="C105" s="20"/>
       <c r="D105" s="21"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>16</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>17</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="9" t="s">
         <v>155</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>43</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>151</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>157</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="39" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A112" s="8" t="s">
         <v>45</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>44</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>160</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
         <v>164</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>162</v>
       </c>
@@ -2910,7 +2910,7 @@
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>34</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>15</v>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>62</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>63</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>41</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="16.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>82</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>83</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="43" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>97</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="43" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>89</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>100</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>101</v>
       </c>
@@ -3054,7 +3054,7 @@
       </c>
       <c r="D127" s="1"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>151</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="100.35" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>131</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>113</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>115</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="16.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>116</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>117</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>121</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>122</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>123</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>124</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>130</v>
       </c>
@@ -3215,7 +3215,7 @@
       </c>
       <c r="D138" s="1"/>
     </row>
-    <row r="139" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="139" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>219</v>
       </c>
@@ -3228,13 +3228,13 @@
       </c>
       <c r="D139" s="1"/>
     </row>
-    <row r="140" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
     </row>
-    <row r="141" spans="1:4" ht="14.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:4" ht="14.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A141" s="19" t="s">
         <v>239</v>
       </c>
@@ -3242,7 +3242,7 @@
       <c r="C141" s="20"/>
       <c r="D141" s="21"/>
     </row>
-    <row r="142" spans="1:4" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="13" t="s">
         <v>227</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="13" t="s">
         <v>229</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="144" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="13" t="s">
         <v>231</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="13" t="s">
         <v>236</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="13" t="s">
         <v>237</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="13" t="s">
         <v>237</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="148" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="13" t="s">
         <v>241</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="149" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="13" t="s">
         <v>242</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="13" t="s">
         <v>248</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="151" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="13" t="s">
         <v>249</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="13" t="s">
         <v>244</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="13" t="s">
         <v>252</v>
       </c>
@@ -3411,49 +3411,49 @@
       </c>
       <c r="D153" s="1"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="13"/>
       <c r="B154" s="13"/>
       <c r="C154" s="13"/>
       <c r="D154" s="1"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="13"/>
       <c r="B155" s="13"/>
       <c r="C155" s="13"/>
       <c r="D155" s="1"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="13"/>
       <c r="B156" s="13"/>
       <c r="C156" s="13"/>
       <c r="D156" s="1"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="13"/>
       <c r="B157" s="13"/>
       <c r="C157" s="13"/>
       <c r="D157" s="1"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="13"/>
       <c r="B158" s="13"/>
       <c r="C158" s="13"/>
       <c r="D158" s="1"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="13"/>
       <c r="B159" s="13"/>
       <c r="C159" s="13"/>
       <c r="D159" s="1"/>
     </row>
-    <row r="160" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A160" s="13"/>
       <c r="B160" s="13"/>
       <c r="C160" s="13"/>
       <c r="D160" s="1"/>
     </row>
-    <row r="161" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A161" s="19" t="s">
         <v>102</v>
       </c>
@@ -3461,7 +3461,7 @@
       <c r="C161" s="20"/>
       <c r="D161" s="21"/>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="162" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>100</v>
       </c>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="D162" s="1"/>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="163" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>135</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="164" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>136</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="165" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>140</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="166" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>139</v>
       </c>
@@ -3532,31 +3532,31 @@
         <v>222</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
     </row>
-    <row r="170" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
     </row>
-    <row r="171" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A171" s="19" t="s">
         <v>149</v>
       </c>
@@ -3564,7 +3564,7 @@
       <c r="C171" s="20"/>
       <c r="D171" s="21"/>
     </row>
-    <row r="172" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="172" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
updated drag buildup excel sheet
</commit_message>
<xml_diff>
--- a/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
+++ b/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bravo_4e3\OneDrive\Documents\GitHub\443_design_problem\drag_buildup_flap_sizing\derivatives\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tysonc/Documents/GitHub/443_design_problem/drag_buildup_flap_sizing/derivatives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5E1F8C-0A3A-435D-9F5C-C163D9D203B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D790720-CE87-5347-A992-065F3F8F58A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{FADF4127-3137-4FB6-88FA-242C48EF07EE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="46280" windowHeight="24040" xr2:uid="{FADF4127-3137-4FB6-88FA-242C48EF07EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Input Equations" sheetId="3" r:id="rId1"/>
@@ -1402,20 +1402,20 @@
   <dimension ref="A1:G172"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H118" sqref="H118"/>
+      <pane ySplit="3" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.234375" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.64453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="2" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>4</v>
       </c>
@@ -1423,7 +1423,7 @@
       <c r="C2" s="23"/>
       <c r="D2" s="24"/>
     </row>
-    <row r="3" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>108</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>143</v>
       </c>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>152</v>
       </c>
@@ -1547,25 +1547,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>53</v>
       </c>
@@ -1573,7 +1573,7 @@
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1711,13 +1711,13 @@
         <v>57</v>
       </c>
       <c r="C25" s="1">
-        <v>8.7759999999999998</v>
+        <v>2.9012129999999998</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -1725,13 +1725,13 @@
         <v>58</v>
       </c>
       <c r="C26" s="1">
-        <v>8.7759999999999998</v>
+        <v>0.16797799999999999</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>59</v>
       </c>
@@ -1739,13 +1739,13 @@
         <v>61</v>
       </c>
       <c r="C27" s="1">
-        <v>8.7759999999999998</v>
+        <v>-8.7759999999999998</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>112</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>113</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>115</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>116</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>117</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>121</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>122</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>123</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>124</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>130</v>
       </c>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>132</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>142</v>
       </c>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>146</v>
       </c>
@@ -1933,19 +1933,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="6"/>
       <c r="C41" s="5"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="6"/>
       <c r="C42" s="5"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>64</v>
       </c>
@@ -1953,7 +1953,7 @@
       <c r="C43" s="20"/>
       <c r="D43" s="21"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="5" t="s">
         <v>30</v>
@@ -2034,7 +2034,7 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
         <v>31</v>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
         <v>32</v>
@@ -2056,7 +2056,7 @@
       </c>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>90</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>91</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>95</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>96</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>224</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>168</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>170</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="86" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>172</v>
       </c>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="1:7" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>174</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>176</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>179</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:7" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>181</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="19" t="s">
         <v>184</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="C64" s="20"/>
       <c r="D64" s="21"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
         <v>5</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="43" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>185</v>
       </c>
@@ -2273,13 +2273,13 @@
         <v>183</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="1:4" ht="16.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:4" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
         <v>187</v>
       </c>
@@ -2287,7 +2287,7 @@
       <c r="C68" s="26"/>
       <c r="D68" s="27"/>
     </row>
-    <row r="69" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>5</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>188</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>189</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="25" t="s">
         <v>192</v>
       </c>
@@ -2339,37 +2339,37 @@
       <c r="C72" s="26"/>
       <c r="D72" s="27"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
       <c r="D73" s="13"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
       <c r="D74" s="13"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
     </row>
-    <row r="77" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>85</v>
       </c>
@@ -2377,7 +2377,7 @@
       <c r="C78" s="20"/>
       <c r="D78" s="21"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>16</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>17</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>78</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>43</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="39" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
         <v>45</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="9" t="s">
         <v>65</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>34</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>15</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>62</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>63</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>41</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>68</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>92</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>94</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="16.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>194</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>113</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>115</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>116</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>117</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>121</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>122</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>123</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>124</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>130</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>131</v>
       </c>
@@ -2740,7 +2740,7 @@
       </c>
       <c r="D103" s="1"/>
     </row>
-    <row r="104" spans="1:4" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>218</v>
       </c>
@@ -2753,7 +2753,7 @@
       </c>
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="19" t="s">
         <v>86</v>
       </c>
@@ -2761,7 +2761,7 @@
       <c r="C105" s="20"/>
       <c r="D105" s="21"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>16</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>17</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="9" t="s">
         <v>155</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>43</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>151</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>157</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="39" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A112" s="8" t="s">
         <v>45</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>44</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>160</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
         <v>164</v>
       </c>
@@ -2894,13 +2894,13 @@
         <v>161</v>
       </c>
       <c r="C115" s="7">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>162</v>
       </c>
@@ -2910,7 +2910,7 @@
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>34</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>15</v>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>62</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>63</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>41</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="16.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>82</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>83</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="43" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>97</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="43" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>89</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>100</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>101</v>
       </c>
@@ -3054,7 +3054,7 @@
       </c>
       <c r="D127" s="1"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>151</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="100.35" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>131</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>113</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>115</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="16.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>116</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>117</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>121</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>122</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>123</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>124</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>130</v>
       </c>
@@ -3215,7 +3215,7 @@
       </c>
       <c r="D138" s="1"/>
     </row>
-    <row r="139" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="139" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>219</v>
       </c>
@@ -3228,13 +3228,13 @@
       </c>
       <c r="D139" s="1"/>
     </row>
-    <row r="140" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
     </row>
-    <row r="141" spans="1:4" ht="14.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:4" ht="14.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A141" s="19" t="s">
         <v>239</v>
       </c>
@@ -3242,7 +3242,7 @@
       <c r="C141" s="20"/>
       <c r="D141" s="21"/>
     </row>
-    <row r="142" spans="1:4" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="13" t="s">
         <v>227</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="13" t="s">
         <v>229</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="144" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="13" t="s">
         <v>231</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="13" t="s">
         <v>236</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="13" t="s">
         <v>237</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="13" t="s">
         <v>237</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="148" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="13" t="s">
         <v>241</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="149" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="13" t="s">
         <v>242</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="13" t="s">
         <v>248</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="151" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="13" t="s">
         <v>249</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="13" t="s">
         <v>244</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="13" t="s">
         <v>252</v>
       </c>
@@ -3411,49 +3411,49 @@
       </c>
       <c r="D153" s="1"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="13"/>
       <c r="B154" s="13"/>
       <c r="C154" s="13"/>
       <c r="D154" s="1"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="13"/>
       <c r="B155" s="13"/>
       <c r="C155" s="13"/>
       <c r="D155" s="1"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="13"/>
       <c r="B156" s="13"/>
       <c r="C156" s="13"/>
       <c r="D156" s="1"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="13"/>
       <c r="B157" s="13"/>
       <c r="C157" s="13"/>
       <c r="D157" s="1"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="13"/>
       <c r="B158" s="13"/>
       <c r="C158" s="13"/>
       <c r="D158" s="1"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="13"/>
       <c r="B159" s="13"/>
       <c r="C159" s="13"/>
       <c r="D159" s="1"/>
     </row>
-    <row r="160" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A160" s="13"/>
       <c r="B160" s="13"/>
       <c r="C160" s="13"/>
       <c r="D160" s="1"/>
     </row>
-    <row r="161" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A161" s="19" t="s">
         <v>102</v>
       </c>
@@ -3461,7 +3461,7 @@
       <c r="C161" s="20"/>
       <c r="D161" s="21"/>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="162" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>100</v>
       </c>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="D162" s="1"/>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="163" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>135</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="164" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>136</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="165" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>140</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="166" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>139</v>
       </c>
@@ -3532,31 +3532,31 @@
         <v>222</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
     </row>
-    <row r="170" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
     </row>
-    <row r="171" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A171" s="19" t="s">
         <v>149</v>
       </c>
@@ -3564,7 +3564,7 @@
       <c r="C171" s="20"/>
       <c r="D171" s="21"/>
     </row>
-    <row r="172" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="172" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
Updated Drag Values (ISR)
</commit_message>
<xml_diff>
--- a/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
+++ b/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tysonc/Documents/GitHub/443_design_problem/drag_buildup_flap_sizing/derivatives/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bravo_4e3\OneDrive\Documents\GitHub\443_design_problem\drag_buildup_flap_sizing\derivatives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D790720-CE87-5347-A992-065F3F8F58A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC973BE2-ACC0-47A0-85AD-C162DBD6C3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="46280" windowHeight="24040" xr2:uid="{FADF4127-3137-4FB6-88FA-242C48EF07EE}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{FADF4127-3137-4FB6-88FA-242C48EF07EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Input Equations" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="260">
   <si>
     <t>S</t>
   </si>
@@ -798,6 +798,24 @@
   </si>
   <si>
     <t>C_D_dropTankWing</t>
+  </si>
+  <si>
+    <t>EO/ISR Drag value</t>
+  </si>
+  <si>
+    <t>C_D_ISR</t>
+  </si>
+  <si>
+    <t>Found through calc</t>
+  </si>
+  <si>
+    <t>area_ISR</t>
+  </si>
+  <si>
+    <t>EO/ISR Area</t>
+  </si>
+  <si>
+    <t>f^2</t>
   </si>
 </sst>
 </file>
@@ -1402,20 +1420,20 @@
   <dimension ref="A1:G172"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I113" sqref="I113"/>
+      <pane ySplit="3" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I153" sqref="I153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.17578125" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.64453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="2" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="22" t="s">
         <v>4</v>
       </c>
@@ -1423,7 +1441,7 @@
       <c r="C2" s="23"/>
       <c r="D2" s="24"/>
     </row>
-    <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
@@ -1437,7 +1455,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1451,7 +1469,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1465,7 +1483,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>108</v>
       </c>
@@ -1479,7 +1497,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
@@ -1493,7 +1511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1507,7 +1525,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1521,7 +1539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>143</v>
       </c>
@@ -1533,7 +1551,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>152</v>
       </c>
@@ -1547,25 +1565,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="19" t="s">
         <v>53</v>
       </c>
@@ -1573,7 +1591,7 @@
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1587,7 +1605,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1601,7 +1619,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1615,7 +1633,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
@@ -1629,7 +1647,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -1644,7 +1662,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
@@ -1659,7 +1677,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1674,7 +1692,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -1689,7 +1707,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -1703,7 +1721,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1717,7 +1735,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -1731,7 +1749,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
         <v>59</v>
       </c>
@@ -1745,7 +1763,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>112</v>
       </c>
@@ -1760,7 +1778,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
         <v>113</v>
       </c>
@@ -1775,7 +1793,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
         <v>115</v>
       </c>
@@ -1790,7 +1808,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
         <v>116</v>
       </c>
@@ -1805,7 +1823,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
         <v>117</v>
       </c>
@@ -1820,7 +1838,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
         <v>121</v>
       </c>
@@ -1835,7 +1853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
         <v>122</v>
       </c>
@@ -1850,7 +1868,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
         <v>123</v>
       </c>
@@ -1865,7 +1883,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
         <v>124</v>
       </c>
@@ -1880,7 +1898,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
         <v>130</v>
       </c>
@@ -1892,7 +1910,7 @@
       </c>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
         <v>132</v>
       </c>
@@ -1906,7 +1924,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
         <v>142</v>
       </c>
@@ -1918,7 +1936,7 @@
       </c>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
         <v>146</v>
       </c>
@@ -1933,19 +1951,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A41" s="1"/>
       <c r="B41" s="6"/>
       <c r="C41" s="5"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1"/>
       <c r="B42" s="6"/>
       <c r="C42" s="5"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="19" t="s">
         <v>64</v>
       </c>
@@ -1953,7 +1971,7 @@
       <c r="C43" s="20"/>
       <c r="D43" s="21"/>
     </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
@@ -1967,7 +1985,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
@@ -1981,7 +1999,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
@@ -1995,7 +2013,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -2009,7 +2027,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
@@ -2023,7 +2041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A49" s="1"/>
       <c r="B49" s="5" t="s">
         <v>30</v>
@@ -2034,7 +2052,7 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
         <v>31</v>
@@ -2045,7 +2063,7 @@
       </c>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
         <v>32</v>
@@ -2056,7 +2074,7 @@
       </c>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A52" s="1" t="s">
         <v>90</v>
       </c>
@@ -2070,7 +2088,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A53" s="1" t="s">
         <v>91</v>
       </c>
@@ -2084,7 +2102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A54" s="1" t="s">
         <v>95</v>
       </c>
@@ -2098,7 +2116,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A55" s="1" t="s">
         <v>96</v>
       </c>
@@ -2112,7 +2130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A56" s="1" t="s">
         <v>224</v>
       </c>
@@ -2129,7 +2147,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A57" s="1" t="s">
         <v>168</v>
       </c>
@@ -2143,7 +2161,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A58" s="1" t="s">
         <v>170</v>
       </c>
@@ -2157,7 +2175,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="86" x14ac:dyDescent="0.5">
       <c r="A59" s="7" t="s">
         <v>172</v>
       </c>
@@ -2169,7 +2187,7 @@
       </c>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A60" s="1" t="s">
         <v>174</v>
       </c>
@@ -2184,7 +2202,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A61" s="1" t="s">
         <v>176</v>
       </c>
@@ -2206,7 +2224,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A62" s="1" t="s">
         <v>179</v>
       </c>
@@ -2221,7 +2239,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
         <v>181</v>
       </c>
@@ -2236,7 +2254,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="19" t="s">
         <v>184</v>
       </c>
@@ -2244,7 +2262,7 @@
       <c r="C64" s="20"/>
       <c r="D64" s="21"/>
     </row>
-    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A65" s="10" t="s">
         <v>5</v>
       </c>
@@ -2258,7 +2276,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="43" x14ac:dyDescent="0.5">
       <c r="A66" s="1" t="s">
         <v>185</v>
       </c>
@@ -2273,13 +2291,13 @@
         <v>183</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="1:4" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="25" t="s">
         <v>187</v>
       </c>
@@ -2287,7 +2305,7 @@
       <c r="C68" s="26"/>
       <c r="D68" s="27"/>
     </row>
-    <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2" t="s">
         <v>5</v>
       </c>
@@ -2301,7 +2319,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A70" s="1" t="s">
         <v>188</v>
       </c>
@@ -2316,7 +2334,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A71" s="1" t="s">
         <v>189</v>
       </c>
@@ -2331,7 +2349,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="25" t="s">
         <v>192</v>
       </c>
@@ -2339,37 +2357,37 @@
       <c r="C72" s="26"/>
       <c r="D72" s="27"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
       <c r="D73" s="13"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
       <c r="D74" s="13"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
     </row>
-    <row r="77" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="19" t="s">
         <v>85</v>
       </c>
@@ -2377,7 +2395,7 @@
       <c r="C78" s="20"/>
       <c r="D78" s="21"/>
     </row>
-    <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A79" s="1" t="s">
         <v>16</v>
       </c>
@@ -2392,7 +2410,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A80" s="1" t="s">
         <v>17</v>
       </c>
@@ -2407,7 +2425,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A81" s="1" t="s">
         <v>78</v>
       </c>
@@ -2421,7 +2439,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A82" s="1" t="s">
         <v>43</v>
       </c>
@@ -2436,7 +2454,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="26" x14ac:dyDescent="0.5">
       <c r="A83" s="8" t="s">
         <v>45</v>
       </c>
@@ -2451,7 +2469,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A84" s="9" t="s">
         <v>65</v>
       </c>
@@ -2465,7 +2483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A85" s="1" t="s">
         <v>34</v>
       </c>
@@ -2480,7 +2498,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A86" s="1" t="s">
         <v>15</v>
       </c>
@@ -2495,7 +2513,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A87" s="1" t="s">
         <v>62</v>
       </c>
@@ -2509,7 +2527,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A88" s="1" t="s">
         <v>63</v>
       </c>
@@ -2523,7 +2541,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A89" s="1" t="s">
         <v>41</v>
       </c>
@@ -2538,7 +2556,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="26" x14ac:dyDescent="0.5">
       <c r="A90" s="1" t="s">
         <v>68</v>
       </c>
@@ -2552,7 +2570,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A91" s="1" t="s">
         <v>92</v>
       </c>
@@ -2566,7 +2584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A92" s="1" t="s">
         <v>94</v>
       </c>
@@ -2580,7 +2598,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A93" s="1" t="s">
         <v>194</v>
       </c>
@@ -2594,7 +2612,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A94" s="1" t="s">
         <v>113</v>
       </c>
@@ -2609,7 +2627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A95" s="1" t="s">
         <v>115</v>
       </c>
@@ -2624,7 +2642,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A96" s="1" t="s">
         <v>116</v>
       </c>
@@ -2639,7 +2657,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A97" s="1" t="s">
         <v>117</v>
       </c>
@@ -2654,7 +2672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A98" s="1" t="s">
         <v>121</v>
       </c>
@@ -2669,7 +2687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A99" s="1" t="s">
         <v>122</v>
       </c>
@@ -2684,7 +2702,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A100" s="1" t="s">
         <v>123</v>
       </c>
@@ -2699,7 +2717,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A101" s="1" t="s">
         <v>124</v>
       </c>
@@ -2714,7 +2732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A102" s="1" t="s">
         <v>130</v>
       </c>
@@ -2728,7 +2746,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A103" s="1" t="s">
         <v>131</v>
       </c>
@@ -2740,7 +2758,7 @@
       </c>
       <c r="D103" s="1"/>
     </row>
-    <row r="104" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1" t="s">
         <v>218</v>
       </c>
@@ -2753,7 +2771,7 @@
       </c>
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="19" t="s">
         <v>86</v>
       </c>
@@ -2761,7 +2779,7 @@
       <c r="C105" s="20"/>
       <c r="D105" s="21"/>
     </row>
-    <row r="106" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A106" s="1" t="s">
         <v>16</v>
       </c>
@@ -2776,7 +2794,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A107" s="1" t="s">
         <v>17</v>
       </c>
@@ -2791,7 +2809,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A108" s="9" t="s">
         <v>155</v>
       </c>
@@ -2805,7 +2823,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A109" s="1" t="s">
         <v>43</v>
       </c>
@@ -2817,7 +2835,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A110" s="1" t="s">
         <v>151</v>
       </c>
@@ -2832,7 +2850,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A111" s="1" t="s">
         <v>157</v>
       </c>
@@ -2846,7 +2864,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" ht="26" x14ac:dyDescent="0.5">
       <c r="A112" s="8" t="s">
         <v>45</v>
       </c>
@@ -2858,7 +2876,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A113" s="1" t="s">
         <v>44</v>
       </c>
@@ -2872,7 +2890,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A114" s="1" t="s">
         <v>160</v>
       </c>
@@ -2886,7 +2904,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A115" s="7" t="s">
         <v>164</v>
       </c>
@@ -2900,7 +2918,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A116" s="1" t="s">
         <v>162</v>
       </c>
@@ -2910,7 +2928,7 @@
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A117" s="1" t="s">
         <v>34</v>
       </c>
@@ -2918,7 +2936,7 @@
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A118" s="1" t="s">
         <v>15</v>
       </c>
@@ -2926,7 +2944,7 @@
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A119" s="1" t="s">
         <v>62</v>
       </c>
@@ -2941,7 +2959,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A120" s="1" t="s">
         <v>63</v>
       </c>
@@ -2956,7 +2974,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A121" s="1" t="s">
         <v>41</v>
       </c>
@@ -2971,7 +2989,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A122" s="1" t="s">
         <v>82</v>
       </c>
@@ -2985,7 +3003,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A123" s="1" t="s">
         <v>83</v>
       </c>
@@ -2999,7 +3017,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="43" x14ac:dyDescent="0.5">
       <c r="A124" s="1" t="s">
         <v>97</v>
       </c>
@@ -3013,7 +3031,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="43" x14ac:dyDescent="0.5">
       <c r="A125" s="1" t="s">
         <v>89</v>
       </c>
@@ -3028,7 +3046,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A126" s="1" t="s">
         <v>100</v>
       </c>
@@ -3042,7 +3060,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A127" s="1" t="s">
         <v>101</v>
       </c>
@@ -3054,7 +3072,7 @@
       </c>
       <c r="D127" s="1"/>
     </row>
-    <row r="128" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A128" s="1" t="s">
         <v>151</v>
       </c>
@@ -3069,7 +3087,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" ht="100.35" x14ac:dyDescent="0.5">
       <c r="A129" s="1" t="s">
         <v>131</v>
       </c>
@@ -3083,7 +3101,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A130" s="1" t="s">
         <v>113</v>
       </c>
@@ -3098,7 +3116,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A131" s="1" t="s">
         <v>115</v>
       </c>
@@ -3113,7 +3131,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A132" s="1" t="s">
         <v>116</v>
       </c>
@@ -3128,7 +3146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A133" s="1" t="s">
         <v>117</v>
       </c>
@@ -3143,7 +3161,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A134" s="1" t="s">
         <v>121</v>
       </c>
@@ -3158,7 +3176,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A135" s="1" t="s">
         <v>122</v>
       </c>
@@ -3173,7 +3191,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A136" s="1" t="s">
         <v>123</v>
       </c>
@@ -3188,7 +3206,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A137" s="1" t="s">
         <v>124</v>
       </c>
@@ -3203,7 +3221,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A138" s="1" t="s">
         <v>130</v>
       </c>
@@ -3215,7 +3233,7 @@
       </c>
       <c r="D138" s="1"/>
     </row>
-    <row r="139" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A139" s="1" t="s">
         <v>219</v>
       </c>
@@ -3228,13 +3246,13 @@
       </c>
       <c r="D139" s="1"/>
     </row>
-    <row r="140" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
     </row>
-    <row r="141" spans="1:4" ht="14.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" ht="14.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="19" t="s">
         <v>239</v>
       </c>
@@ -3242,7 +3260,7 @@
       <c r="C141" s="20"/>
       <c r="D141" s="21"/>
     </row>
-    <row r="142" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A142" s="13" t="s">
         <v>227</v>
       </c>
@@ -3256,7 +3274,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A143" s="13" t="s">
         <v>229</v>
       </c>
@@ -3271,7 +3289,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A144" s="13" t="s">
         <v>231</v>
       </c>
@@ -3285,7 +3303,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A145" s="13" t="s">
         <v>236</v>
       </c>
@@ -3299,7 +3317,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A146" s="13" t="s">
         <v>237</v>
       </c>
@@ -3313,7 +3331,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A147" s="13" t="s">
         <v>237</v>
       </c>
@@ -3327,7 +3345,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A148" s="13" t="s">
         <v>241</v>
       </c>
@@ -3341,7 +3359,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A149" s="13" t="s">
         <v>242</v>
       </c>
@@ -3356,7 +3374,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A150" s="13" t="s">
         <v>248</v>
       </c>
@@ -3370,7 +3388,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A151" s="13" t="s">
         <v>249</v>
       </c>
@@ -3385,7 +3403,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A152" s="13" t="s">
         <v>244</v>
       </c>
@@ -3399,7 +3417,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A153" s="13" t="s">
         <v>252</v>
       </c>
@@ -3411,49 +3429,66 @@
       </c>
       <c r="D153" s="1"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A154" s="13"/>
-      <c r="B154" s="13"/>
-      <c r="C154" s="13"/>
-      <c r="D154" s="1"/>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A155" s="13"/>
-      <c r="B155" s="13"/>
-      <c r="C155" s="13"/>
-      <c r="D155" s="1"/>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" ht="43" x14ac:dyDescent="0.5">
+      <c r="A154" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="B154" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="C154" s="13">
+        <v>0.68</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A155" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="B155" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C155" s="13">
+        <f>((3.14*(14^2)/4)/2 + (8.5*14))/144</f>
+        <v>1.360625</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A156" s="13"/>
       <c r="B156" s="13"/>
       <c r="C156" s="13"/>
       <c r="D156" s="1"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A157" s="13"/>
       <c r="B157" s="13"/>
       <c r="C157" s="13"/>
       <c r="D157" s="1"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A158" s="13"/>
       <c r="B158" s="13"/>
       <c r="C158" s="13"/>
       <c r="D158" s="1"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A159" s="13"/>
       <c r="B159" s="13"/>
       <c r="C159" s="13"/>
       <c r="D159" s="1"/>
     </row>
-    <row r="160" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="13"/>
       <c r="B160" s="13"/>
       <c r="C160" s="13"/>
       <c r="D160" s="1"/>
     </row>
-    <row r="161" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="19" t="s">
         <v>102</v>
       </c>
@@ -3461,7 +3496,7 @@
       <c r="C161" s="20"/>
       <c r="D161" s="21"/>
     </row>
-    <row r="162" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A162" s="1" t="s">
         <v>100</v>
       </c>
@@ -3473,7 +3508,7 @@
       </c>
       <c r="D162" s="1"/>
     </row>
-    <row r="163" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A163" s="1" t="s">
         <v>135</v>
       </c>
@@ -3487,7 +3522,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A164" s="1" t="s">
         <v>136</v>
       </c>
@@ -3501,7 +3536,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" ht="43" x14ac:dyDescent="0.5">
       <c r="A165" s="1" t="s">
         <v>140</v>
       </c>
@@ -3515,7 +3550,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" ht="43" x14ac:dyDescent="0.5">
       <c r="A166" s="1" t="s">
         <v>139</v>
       </c>
@@ -3532,31 +3567,31 @@
         <v>222</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
     </row>
-    <row r="170" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
     </row>
-    <row r="171" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="19" t="s">
         <v>149</v>
       </c>
@@ -3564,7 +3599,7 @@
       <c r="C171" s="20"/>
       <c r="D171" s="21"/>
     </row>
-    <row r="172" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A172" s="1" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
Drag update 2 for new fuel mission
</commit_message>
<xml_diff>
--- a/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
+++ b/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bravo_4e3\OneDrive\Documents\GitHub\443_design_problem\drag_buildup_flap_sizing\derivatives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC973BE2-ACC0-47A0-85AD-C162DBD6C3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B4281C-A6A0-4675-B89D-D9B362DD792A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{FADF4127-3137-4FB6-88FA-242C48EF07EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="264">
   <si>
     <t>S</t>
   </si>
@@ -816,6 +816,18 @@
   </si>
   <si>
     <t>f^2</t>
+  </si>
+  <si>
+    <t>120 gal drop tank</t>
+  </si>
+  <si>
+    <t>area120DropTank</t>
+  </si>
+  <si>
+    <t>120 gal drop tank d</t>
+  </si>
+  <si>
+    <t>d_120dropTank</t>
   </si>
 </sst>
 </file>
@@ -1417,11 +1429,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5E94DD-475C-4C1A-B69B-A897EE12FF00}">
-  <dimension ref="A1:G172"/>
+  <dimension ref="A1:G174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I153" sqref="I153"/>
+      <pane ySplit="3" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3429,46 +3441,65 @@
       </c>
       <c r="D153" s="1"/>
     </row>
-    <row r="154" spans="1:4" ht="43" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A154" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="B154" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="C154">
+        <f>11.7*2</f>
+        <v>23.4</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A155" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="B155" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="C155" s="13">
+        <f>((C154^2 *PI())/4)/144</f>
+        <v>2.9864765163187967</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="43" x14ac:dyDescent="0.5">
+      <c r="A156" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="B154" s="13" t="s">
+      <c r="B156" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="C154" s="13">
-        <v>0.68</v>
-      </c>
-      <c r="D154" s="1" t="s">
+      <c r="C156" s="13">
+        <f>0.58+0.1</f>
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="D156" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A155" s="13" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A157" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="B155" s="13" t="s">
+      <c r="B157" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C155" s="13">
+      <c r="C157" s="13">
         <f>((3.14*(14^2)/4)/2 + (8.5*14))/144</f>
         <v>1.360625</v>
       </c>
-      <c r="D155" s="1" t="s">
+      <c r="D157" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A156" s="13"/>
-      <c r="B156" s="13"/>
-      <c r="C156" s="13"/>
-      <c r="D156" s="1"/>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A157" s="13"/>
-      <c r="B157" s="13"/>
-      <c r="C157" s="13"/>
-      <c r="D157" s="1"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A158" s="13"/>
@@ -3482,102 +3513,102 @@
       <c r="C159" s="13"/>
       <c r="D159" s="1"/>
     </row>
-    <row r="160" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A160" s="13"/>
       <c r="B160" s="13"/>
       <c r="C160" s="13"/>
       <c r="D160" s="1"/>
     </row>
-    <row r="161" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A161" s="19" t="s">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A161" s="13"/>
+      <c r="B161" s="13"/>
+      <c r="C161" s="13"/>
+      <c r="D161" s="1"/>
+    </row>
+    <row r="162" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162" s="13"/>
+      <c r="B162" s="13"/>
+      <c r="C162" s="13"/>
+      <c r="D162" s="1"/>
+    </row>
+    <row r="163" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B161" s="20"/>
-      <c r="C161" s="20"/>
-      <c r="D161" s="21"/>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A162" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C162" s="1">
-        <v>0</v>
-      </c>
-      <c r="D162" s="1"/>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A163" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B163" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C163" s="1">
-        <v>-10</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="B163" s="20"/>
+      <c r="C163" s="20"/>
+      <c r="D163" s="21"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A164" s="1" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="C164" s="1">
-        <v>12</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+        <v>0</v>
+      </c>
+      <c r="D164" s="1"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A165" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+      <c r="B165" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="C165" s="1">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A166" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C166" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F166" s="1" t="s">
+    </row>
+    <row r="167" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A167" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C167" s="1">
+        <v>-5</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A168" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C168" s="1">
+        <v>2</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F168" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A167" s="1"/>
-      <c r="B167" s="1"/>
-      <c r="C167" s="1"/>
-      <c r="D167" s="1"/>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A168" s="1"/>
-      <c r="B168" s="1"/>
-      <c r="C168" s="1"/>
-      <c r="D168" s="1"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A169" s="1"/>
@@ -3585,36 +3616,48 @@
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
     </row>
-    <row r="170" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
     </row>
-    <row r="171" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A171" s="19" t="s">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+    </row>
+    <row r="172" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
+      <c r="C172" s="1"/>
+      <c r="D172" s="1"/>
+    </row>
+    <row r="173" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A173" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="B171" s="20"/>
-      <c r="C171" s="20"/>
-      <c r="D171" s="21"/>
-    </row>
-    <row r="172" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A172" s="1" t="s">
+      <c r="B173" s="20"/>
+      <c r="C173" s="20"/>
+      <c r="D173" s="21"/>
+    </row>
+    <row r="174" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A174" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B172" s="1" t="s">
+      <c r="B174" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C172" s="1">
+      <c r="C174" s="1">
         <v>0</v>
       </c>
-      <c r="D172" s="1"/>
+      <c r="D174" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A171:D171"/>
-    <mergeCell ref="A161:D161"/>
+    <mergeCell ref="A173:D173"/>
+    <mergeCell ref="A163:D163"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A43:D43"/>

</xml_diff>

<commit_message>
drag update iwht the fuel
</commit_message>
<xml_diff>
--- a/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
+++ b/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tysonc/Documents/GitHub/443_design_problem/drag_buildup_flap_sizing/derivatives/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bravo_4e3\OneDrive\Documents\GitHub\443_design_problem\drag_buildup_flap_sizing\derivatives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A5DB26-0F60-D64E-8864-F48380F65570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30BB4A5-ACDB-4C0B-ACEF-7FE772123CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17120" yWindow="3860" windowWidth="34560" windowHeight="21580" xr2:uid="{FADF4127-3137-4FB6-88FA-242C48EF07EE}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{FADF4127-3137-4FB6-88FA-242C48EF07EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Input Equations" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="273">
   <si>
     <t>S</t>
   </si>
@@ -843,6 +843,18 @@
   </si>
   <si>
     <t>assuming c_barbar_i = S_i/b_i</t>
+  </si>
+  <si>
+    <t>d_175dropTank</t>
+  </si>
+  <si>
+    <t>area175DropTank</t>
+  </si>
+  <si>
+    <t>175 gal drop tank d</t>
+  </si>
+  <si>
+    <t>175 gal drop tank</t>
   </si>
 </sst>
 </file>
@@ -893,6 +905,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1444,23 +1457,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5E94DD-475C-4C1A-B69B-A897EE12FF00}">
-  <dimension ref="A1:G174"/>
+  <dimension ref="A1:G173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <pane ySplit="3" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I153" sqref="I153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.17578125" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.64453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="2" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="22" t="s">
         <v>4</v>
       </c>
@@ -1468,7 +1481,7 @@
       <c r="C2" s="23"/>
       <c r="D2" s="24"/>
     </row>
-    <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
@@ -1482,7 +1495,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1496,7 +1509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1510,7 +1523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>108</v>
       </c>
@@ -1524,7 +1537,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
@@ -1538,7 +1551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1552,7 +1565,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1566,7 +1579,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>143</v>
       </c>
@@ -1578,7 +1591,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>152</v>
       </c>
@@ -1592,25 +1605,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="19" t="s">
         <v>53</v>
       </c>
@@ -1618,7 +1631,7 @@
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1632,7 +1645,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1646,7 +1659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1660,7 +1673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
@@ -1674,7 +1687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -1689,7 +1702,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
@@ -1704,7 +1717,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1719,7 +1732,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -1734,7 +1747,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -1748,7 +1761,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1762,7 +1775,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -1776,7 +1789,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
         <v>59</v>
       </c>
@@ -1790,7 +1803,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>112</v>
       </c>
@@ -1805,7 +1818,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
         <v>113</v>
       </c>
@@ -1819,7 +1832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
         <v>115</v>
       </c>
@@ -1833,7 +1846,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
         <v>116</v>
       </c>
@@ -1847,7 +1860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
         <v>117</v>
       </c>
@@ -1861,7 +1874,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
         <v>264</v>
       </c>
@@ -1876,7 +1889,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
         <v>265</v>
       </c>
@@ -1891,7 +1904,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
         <v>266</v>
       </c>
@@ -1909,7 +1922,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
         <v>267</v>
       </c>
@@ -1924,7 +1937,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
         <v>130</v>
       </c>
@@ -1936,7 +1949,7 @@
       </c>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
         <v>132</v>
       </c>
@@ -1950,7 +1963,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
         <v>142</v>
       </c>
@@ -1962,7 +1975,7 @@
       </c>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
         <v>146</v>
       </c>
@@ -1977,19 +1990,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A41" s="1"/>
       <c r="B41" s="6"/>
       <c r="C41" s="5"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1"/>
       <c r="B42" s="6"/>
       <c r="C42" s="5"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="19" t="s">
         <v>64</v>
       </c>
@@ -1997,7 +2010,7 @@
       <c r="C43" s="20"/>
       <c r="D43" s="21"/>
     </row>
-    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
@@ -2011,7 +2024,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
@@ -2025,7 +2038,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
@@ -2039,7 +2052,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -2053,7 +2066,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
@@ -2067,7 +2080,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A49" s="1"/>
       <c r="B49" s="5" t="s">
         <v>30</v>
@@ -2078,7 +2091,7 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
         <v>31</v>
@@ -2089,7 +2102,7 @@
       </c>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
         <v>32</v>
@@ -2100,7 +2113,7 @@
       </c>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A52" s="1" t="s">
         <v>90</v>
       </c>
@@ -2114,7 +2127,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A53" s="1" t="s">
         <v>91</v>
       </c>
@@ -2128,7 +2141,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A54" s="1" t="s">
         <v>95</v>
       </c>
@@ -2142,7 +2155,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A55" s="1" t="s">
         <v>96</v>
       </c>
@@ -2156,7 +2169,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A56" s="1" t="s">
         <v>224</v>
       </c>
@@ -2173,7 +2186,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A57" s="1" t="s">
         <v>168</v>
       </c>
@@ -2187,7 +2200,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A58" s="1" t="s">
         <v>170</v>
       </c>
@@ -2201,7 +2214,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="86" x14ac:dyDescent="0.5">
       <c r="A59" s="7" t="s">
         <v>172</v>
       </c>
@@ -2213,7 +2226,7 @@
       </c>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A60" s="1" t="s">
         <v>174</v>
       </c>
@@ -2228,7 +2241,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A61" s="1" t="s">
         <v>176</v>
       </c>
@@ -2250,7 +2263,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A62" s="1" t="s">
         <v>179</v>
       </c>
@@ -2265,7 +2278,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
         <v>181</v>
       </c>
@@ -2280,7 +2293,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="19" t="s">
         <v>184</v>
       </c>
@@ -2288,7 +2301,7 @@
       <c r="C64" s="20"/>
       <c r="D64" s="21"/>
     </row>
-    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A65" s="10" t="s">
         <v>5</v>
       </c>
@@ -2302,7 +2315,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="43" x14ac:dyDescent="0.5">
       <c r="A66" s="1" t="s">
         <v>185</v>
       </c>
@@ -2317,13 +2330,13 @@
         <v>183</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="1:4" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="25" t="s">
         <v>187</v>
       </c>
@@ -2331,7 +2344,7 @@
       <c r="C68" s="26"/>
       <c r="D68" s="27"/>
     </row>
-    <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2" t="s">
         <v>5</v>
       </c>
@@ -2345,7 +2358,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A70" s="1" t="s">
         <v>188</v>
       </c>
@@ -2360,7 +2373,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A71" s="1" t="s">
         <v>189</v>
       </c>
@@ -2375,7 +2388,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="25" t="s">
         <v>192</v>
       </c>
@@ -2383,37 +2396,37 @@
       <c r="C72" s="26"/>
       <c r="D72" s="27"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
       <c r="D73" s="13"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
       <c r="D74" s="13"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
     </row>
-    <row r="77" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="19" t="s">
         <v>85</v>
       </c>
@@ -2421,7 +2434,7 @@
       <c r="C78" s="20"/>
       <c r="D78" s="21"/>
     </row>
-    <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A79" s="1" t="s">
         <v>16</v>
       </c>
@@ -2436,7 +2449,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A80" s="1" t="s">
         <v>17</v>
       </c>
@@ -2451,7 +2464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A81" s="1" t="s">
         <v>78</v>
       </c>
@@ -2465,7 +2478,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A82" s="1" t="s">
         <v>43</v>
       </c>
@@ -2480,7 +2493,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="26" x14ac:dyDescent="0.5">
       <c r="A83" s="8" t="s">
         <v>45</v>
       </c>
@@ -2495,7 +2508,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A84" s="9" t="s">
         <v>65</v>
       </c>
@@ -2509,7 +2522,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A85" s="1" t="s">
         <v>34</v>
       </c>
@@ -2524,7 +2537,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A86" s="1" t="s">
         <v>15</v>
       </c>
@@ -2539,7 +2552,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A87" s="1" t="s">
         <v>62</v>
       </c>
@@ -2553,7 +2566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A88" s="1" t="s">
         <v>63</v>
       </c>
@@ -2567,7 +2580,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A89" s="1" t="s">
         <v>41</v>
       </c>
@@ -2582,7 +2595,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="26" x14ac:dyDescent="0.5">
       <c r="A90" s="1" t="s">
         <v>68</v>
       </c>
@@ -2596,7 +2609,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A91" s="1" t="s">
         <v>92</v>
       </c>
@@ -2610,7 +2623,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A92" s="1" t="s">
         <v>94</v>
       </c>
@@ -2624,7 +2637,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A93" s="1" t="s">
         <v>194</v>
       </c>
@@ -2638,7 +2651,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A94" s="1" t="s">
         <v>113</v>
       </c>
@@ -2653,7 +2666,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A95" s="1" t="s">
         <v>115</v>
       </c>
@@ -2668,7 +2681,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A96" s="1" t="s">
         <v>116</v>
       </c>
@@ -2683,7 +2696,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A97" s="1" t="s">
         <v>117</v>
       </c>
@@ -2698,7 +2711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A98" s="1" t="s">
         <v>121</v>
       </c>
@@ -2713,7 +2726,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A99" s="1" t="s">
         <v>122</v>
       </c>
@@ -2728,7 +2741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A100" s="1" t="s">
         <v>123</v>
       </c>
@@ -2743,7 +2756,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A101" s="1" t="s">
         <v>124</v>
       </c>
@@ -2758,7 +2771,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A102" s="1" t="s">
         <v>130</v>
       </c>
@@ -2772,7 +2785,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A103" s="1" t="s">
         <v>131</v>
       </c>
@@ -2784,7 +2797,7 @@
       </c>
       <c r="D103" s="1"/>
     </row>
-    <row r="104" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1" t="s">
         <v>218</v>
       </c>
@@ -2797,7 +2810,7 @@
       </c>
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="19" t="s">
         <v>86</v>
       </c>
@@ -2805,7 +2818,7 @@
       <c r="C105" s="20"/>
       <c r="D105" s="21"/>
     </row>
-    <row r="106" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A106" s="1" t="s">
         <v>16</v>
       </c>
@@ -2820,7 +2833,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A107" s="1" t="s">
         <v>17</v>
       </c>
@@ -2835,7 +2848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A108" s="9" t="s">
         <v>155</v>
       </c>
@@ -2849,7 +2862,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A109" s="1" t="s">
         <v>43</v>
       </c>
@@ -2861,7 +2874,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A110" s="1" t="s">
         <v>151</v>
       </c>
@@ -2876,7 +2889,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A111" s="1" t="s">
         <v>157</v>
       </c>
@@ -2890,7 +2903,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" ht="26" x14ac:dyDescent="0.5">
       <c r="A112" s="8" t="s">
         <v>45</v>
       </c>
@@ -2902,7 +2915,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A113" s="1" t="s">
         <v>44</v>
       </c>
@@ -2916,7 +2929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A114" s="1" t="s">
         <v>160</v>
       </c>
@@ -2930,7 +2943,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A115" s="7" t="s">
         <v>164</v>
       </c>
@@ -2944,7 +2957,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A116" s="1" t="s">
         <v>162</v>
       </c>
@@ -2954,7 +2967,7 @@
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A117" s="1" t="s">
         <v>34</v>
       </c>
@@ -2962,7 +2975,7 @@
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A118" s="1" t="s">
         <v>15</v>
       </c>
@@ -2970,7 +2983,7 @@
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A119" s="1" t="s">
         <v>62</v>
       </c>
@@ -2985,7 +2998,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A120" s="1" t="s">
         <v>63</v>
       </c>
@@ -3000,7 +3013,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A121" s="1" t="s">
         <v>41</v>
       </c>
@@ -3015,7 +3028,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A122" s="1" t="s">
         <v>82</v>
       </c>
@@ -3029,7 +3042,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A123" s="1" t="s">
         <v>83</v>
       </c>
@@ -3043,7 +3056,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="43" x14ac:dyDescent="0.5">
       <c r="A124" s="1" t="s">
         <v>97</v>
       </c>
@@ -3057,7 +3070,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="43" x14ac:dyDescent="0.5">
       <c r="A125" s="1" t="s">
         <v>89</v>
       </c>
@@ -3072,7 +3085,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A126" s="1" t="s">
         <v>100</v>
       </c>
@@ -3086,7 +3099,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A127" s="1" t="s">
         <v>101</v>
       </c>
@@ -3098,7 +3111,7 @@
       </c>
       <c r="D127" s="1"/>
     </row>
-    <row r="128" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A128" s="1" t="s">
         <v>151</v>
       </c>
@@ -3113,7 +3126,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" ht="100.35" x14ac:dyDescent="0.5">
       <c r="A129" s="1" t="s">
         <v>131</v>
       </c>
@@ -3127,7 +3140,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A130" s="1" t="s">
         <v>113</v>
       </c>
@@ -3142,7 +3155,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A131" s="1" t="s">
         <v>115</v>
       </c>
@@ -3157,7 +3170,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A132" s="1" t="s">
         <v>116</v>
       </c>
@@ -3172,7 +3185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A133" s="1" t="s">
         <v>117</v>
       </c>
@@ -3187,7 +3200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A134" s="1" t="s">
         <v>121</v>
       </c>
@@ -3202,7 +3215,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A135" s="1" t="s">
         <v>122</v>
       </c>
@@ -3217,7 +3230,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A136" s="1" t="s">
         <v>123</v>
       </c>
@@ -3232,7 +3245,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A137" s="1" t="s">
         <v>124</v>
       </c>
@@ -3247,7 +3260,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A138" s="1" t="s">
         <v>130</v>
       </c>
@@ -3259,7 +3272,7 @@
       </c>
       <c r="D138" s="1"/>
     </row>
-    <row r="139" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A139" s="1" t="s">
         <v>219</v>
       </c>
@@ -3272,13 +3285,13 @@
       </c>
       <c r="D139" s="1"/>
     </row>
-    <row r="140" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
     </row>
-    <row r="141" spans="1:4" ht="14.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" ht="14.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="19" t="s">
         <v>239</v>
       </c>
@@ -3286,7 +3299,7 @@
       <c r="C141" s="20"/>
       <c r="D141" s="21"/>
     </row>
-    <row r="142" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A142" s="13" t="s">
         <v>227</v>
       </c>
@@ -3300,7 +3313,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A143" s="13" t="s">
         <v>229</v>
       </c>
@@ -3315,7 +3328,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A144" s="13" t="s">
         <v>231</v>
       </c>
@@ -3329,7 +3342,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A145" s="13" t="s">
         <v>236</v>
       </c>
@@ -3343,7 +3356,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A146" s="13" t="s">
         <v>237</v>
       </c>
@@ -3357,7 +3370,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A147" s="13" t="s">
         <v>237</v>
       </c>
@@ -3371,7 +3384,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A148" s="13" t="s">
         <v>241</v>
       </c>
@@ -3385,7 +3398,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A149" s="13" t="s">
         <v>242</v>
       </c>
@@ -3400,7 +3413,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A150" s="13" t="s">
         <v>248</v>
       </c>
@@ -3414,7 +3427,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A151" s="13" t="s">
         <v>249</v>
       </c>
@@ -3429,7 +3442,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A152" s="13" t="s">
         <v>244</v>
       </c>
@@ -3443,7 +3456,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A153" s="13" t="s">
         <v>252</v>
       </c>
@@ -3455,7 +3468,7 @@
       </c>
       <c r="D153" s="1"/>
     </row>
-    <row r="154" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A154" s="13" t="s">
         <v>262</v>
       </c>
@@ -3470,7 +3483,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A155" s="13" t="s">
         <v>260</v>
       </c>
@@ -3485,193 +3498,204 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A156" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="B156" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="C156" s="13">
+        <v>27</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A157" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="B157" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="C157" s="13">
+        <f>((C156^2 *PI())/4)/144</f>
+        <v>3.9760782021995817</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="43" x14ac:dyDescent="0.5">
+      <c r="A158" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="B156" s="13" t="s">
+      <c r="B158" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="C156" s="13">
+      <c r="C158" s="13">
         <f>0.58+0.1</f>
         <v>0.67999999999999994</v>
       </c>
-      <c r="D156" s="1" t="s">
+      <c r="D158" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A157" s="13" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A159" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="B157" s="13" t="s">
+      <c r="B159" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C157" s="13">
+      <c r="C159" s="13">
         <f>((3.14*(14^2)/4)/2 + (8.5*14))/144</f>
         <v>1.360625</v>
       </c>
-      <c r="D157" s="1" t="s">
+      <c r="D159" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A158" s="13"/>
-      <c r="B158" s="13"/>
-      <c r="C158" s="13"/>
-      <c r="D158" s="1"/>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A159" s="13"/>
-      <c r="B159" s="13"/>
-      <c r="C159" s="13"/>
-      <c r="D159" s="1"/>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A160" s="13"/>
       <c r="B160" s="13"/>
       <c r="C160" s="13"/>
       <c r="D160" s="1"/>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="13"/>
       <c r="B161" s="13"/>
       <c r="C161" s="13"/>
       <c r="D161" s="1"/>
     </row>
-    <row r="162" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="13"/>
-      <c r="B162" s="13"/>
-      <c r="C162" s="13"/>
-      <c r="D162" s="1"/>
-    </row>
-    <row r="163" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="19" t="s">
+    <row r="162" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B163" s="20"/>
-      <c r="C163" s="20"/>
-      <c r="D163" s="21"/>
-    </row>
-    <row r="164" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B162" s="20"/>
+      <c r="C162" s="20"/>
+      <c r="D162" s="21"/>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A163" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C163" s="1">
+        <v>0</v>
+      </c>
+      <c r="D163" s="1"/>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A164" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>99</v>
+        <v>135</v>
+      </c>
+      <c r="B164" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="C164" s="1">
-        <v>0</v>
-      </c>
-      <c r="D164" s="1"/>
-    </row>
-    <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>-10</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A165" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B165" s="6" t="s">
-        <v>133</v>
+        <v>136</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="C165" s="1">
-        <v>-10</v>
+        <v>12</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" ht="43" x14ac:dyDescent="0.5">
       <c r="A166" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C166" s="1">
-        <v>12</v>
+        <v>-5</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" ht="43" x14ac:dyDescent="0.5">
       <c r="A167" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C167" s="1">
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A168" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C168" s="1">
-        <v>2</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F168" s="1" t="s">
+      <c r="F167" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1"/>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
     </row>
-    <row r="172" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="1"/>
-      <c r="B172" s="1"/>
-      <c r="C172" s="1"/>
-      <c r="D172" s="1"/>
-    </row>
-    <row r="173" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="19" t="s">
+    <row r="172" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A172" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="B173" s="20"/>
-      <c r="C173" s="20"/>
-      <c r="D173" s="21"/>
-    </row>
-    <row r="174" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A174" s="1" t="s">
+      <c r="B172" s="20"/>
+      <c r="C172" s="20"/>
+      <c r="D172" s="21"/>
+    </row>
+    <row r="173" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A173" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B174" s="1" t="s">
+      <c r="B173" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C174" s="1">
+      <c r="C173" s="1">
         <v>0</v>
       </c>
-      <c r="D174" s="1"/>
+      <c r="D173" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A173:D173"/>
-    <mergeCell ref="A163:D163"/>
+    <mergeCell ref="A172:D172"/>
+    <mergeCell ref="A162:D162"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A43:D43"/>

</xml_diff>

<commit_message>
Calculated Drag for different munitions
</commit_message>
<xml_diff>
--- a/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
+++ b/drag_buildup_flap_sizing/derivatives/DragBuildUp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bravo_4e3\OneDrive\Documents\GitHub\443_design_problem\drag_buildup_flap_sizing\derivatives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B33F5E9-03F8-4955-A844-DDF5A5CD6473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1013E83B-E715-46B6-BF59-8572428EA985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{FADF4127-3137-4FB6-88FA-242C48EF07EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="285">
   <si>
     <t>S</t>
   </si>
@@ -876,6 +876,21 @@
   </si>
   <si>
     <t>2D area of AIM9</t>
+  </si>
+  <si>
+    <t>2D area of AGM114</t>
+  </si>
+  <si>
+    <t>d_AGM114</t>
+  </si>
+  <si>
+    <t>AGM114 diameter</t>
+  </si>
+  <si>
+    <t>area_AGM114</t>
+  </si>
+  <si>
+    <t>area_AIM9</t>
   </si>
 </sst>
 </file>
@@ -1481,8 +1496,8 @@
   <dimension ref="A1:G181"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H174" sqref="H174"/>
+      <pane ySplit="3" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F148" sqref="F148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3453,7 +3468,7 @@
         <v>279</v>
       </c>
       <c r="B151" s="18" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="C151" s="13">
         <f>((C150^2 *PI())/4)/144</f>
@@ -3463,7 +3478,35 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="152" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A152" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="B152" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="C152">
+        <v>7</v>
+      </c>
+      <c r="D152" s="13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A153" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="B153" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="C153" s="13">
+        <f>((C152^2 *PI())/4)/144</f>
+        <v>0.26725354171163168</v>
+      </c>
+      <c r="D153" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A157" s="13" t="s">
         <v>241</v>

</xml_diff>